<commit_message>
added more wage gap related files to 290
</commit_message>
<xml_diff>
--- a/CSS290/SDR2015_DST_50.xlsx
+++ b/CSS290/SDR2015_DST_50.xlsx
@@ -3,15 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF9FEFAA-FDD1-435E-A901-5B1F158219F4}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A102B0E6-E65C-4AE1-9E02-4FF21C549A36}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23640" windowHeight="12480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23640" windowHeight="12480" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet6" sheetId="7" r:id="rId1"/>
-    <sheet name="Graph Sheet" sheetId="9" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId3"/>
-    <sheet name="SDR2015_DST_50" sheetId="1" r:id="rId4"/>
+    <sheet name="Graph Data Analysis Tables" sheetId="7" r:id="rId1"/>
+    <sheet name="Graphs" sheetId="9" r:id="rId2"/>
+    <sheet name="Raw_Data_restructured" sheetId="2" r:id="rId3"/>
+    <sheet name="Raw_Data_Sheet" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
   <pivotCaches>
@@ -5704,7 +5704,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[SDR2015_DST_50.xlsx]Sheet6!PivotTable9</c:name>
+    <c:name>[SDR2015_DST_50.xlsx]Graph Data Analysis Tables!PivotTable9</c:name>
     <c:fmtId val="3"/>
   </c:pivotSource>
   <c:chart>
@@ -6526,7 +6526,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet6!$B$3</c:f>
+              <c:f>'Graph Data Analysis Tables'!$B$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6561,7 +6561,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet6!$A$4:$A$29</c:f>
+              <c:f>'Graph Data Analysis Tables'!$A$4:$A$29</c:f>
               <c:strCache>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
@@ -6647,7 +6647,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet6!$B$4:$B$29</c:f>
+              <c:f>'Graph Data Analysis Tables'!$B$4:$B$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
@@ -6744,7 +6744,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet6!$C$3</c:f>
+              <c:f>'Graph Data Analysis Tables'!$C$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6779,7 +6779,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet6!$A$4:$A$29</c:f>
+              <c:f>'Graph Data Analysis Tables'!$A$4:$A$29</c:f>
               <c:strCache>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
@@ -6865,7 +6865,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet6!$C$4:$C$29</c:f>
+              <c:f>'Graph Data Analysis Tables'!$C$4:$C$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
@@ -6962,7 +6962,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet6!$D$3</c:f>
+              <c:f>'Graph Data Analysis Tables'!$D$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6997,7 +6997,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet6!$A$4:$A$29</c:f>
+              <c:f>'Graph Data Analysis Tables'!$A$4:$A$29</c:f>
               <c:strCache>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
@@ -7083,7 +7083,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet6!$D$4:$D$29</c:f>
+              <c:f>'Graph Data Analysis Tables'!$D$4:$D$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
@@ -7180,7 +7180,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet6!$E$3</c:f>
+              <c:f>'Graph Data Analysis Tables'!$E$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -7215,7 +7215,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet6!$A$4:$A$29</c:f>
+              <c:f>'Graph Data Analysis Tables'!$A$4:$A$29</c:f>
               <c:strCache>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
@@ -7301,7 +7301,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet6!$E$4:$E$29</c:f>
+              <c:f>'Graph Data Analysis Tables'!$E$4:$E$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
@@ -7398,7 +7398,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet6!$F$3</c:f>
+              <c:f>'Graph Data Analysis Tables'!$F$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -7433,7 +7433,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet6!$A$4:$A$29</c:f>
+              <c:f>'Graph Data Analysis Tables'!$A$4:$A$29</c:f>
               <c:strCache>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
@@ -7519,7 +7519,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet6!$F$4:$F$29</c:f>
+              <c:f>'Graph Data Analysis Tables'!$F$4:$F$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
@@ -7848,8 +7848,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.77772092003580762"/>
           <c:y val="0.91182110916690984"/>
-          <c:w val="0.22227905969994083"/>
-          <c:h val="8.8178890833090315E-2"/>
+          <c:w val="0.22227913338605781"/>
+          <c:h val="8.8178973024306037E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -7975,16 +7975,53 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Industries ordered from left to right</a:t>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>Industries are sorted descending order, from left to right, according to: </a:t>
             </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US" baseline="0"/>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> as those with greatest % of total population as women, to least % of total population as women</a:t>
+              <a:t>Female Per-Industry Median Salary as a % of Male all-industry averaged median salary </a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>DIVIDED by </a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>Male Per-Industry Median Salary as a % of Male all-industry averaged median Salary </a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.12132638319365004"/>
+          <c:y val="0"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8017,16 +8054,15 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet6!$C$39</c:f>
+              <c:f>'Graph Data Analysis Tables'!$C$39</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -8036,99 +8072,117 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln w="25400">
-              <a:noFill/>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet6!$A$39:$A$65</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Graph Data Analysis Tables'!$A$39:$A$65</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'Graph Data Analysis Tables'!$A$40:$A$65</c:f>
               <c:strCache>
-                <c:ptCount val="27"/>
+                <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>Row Labels</c:v>
+                  <c:v>Sociology</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Sociology</c:v>
+                  <c:v>Mechanical engineering</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Mechanical engineering</c:v>
+                  <c:v>Aerospace/aeronautical/astronautical engineering</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Aerospace/aeronautical/astronautical engineering</c:v>
+                  <c:v>Political sciences</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Political sciences</c:v>
+                  <c:v>Materials and metallurgical engineering</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Materials and metallurgical engineering</c:v>
+                  <c:v>Mathematics/statistics</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Mathematics/statistics</c:v>
+                  <c:v>Chemical engineering</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Chemical engineering</c:v>
+                  <c:v>Electrical/computer engineering</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Electrical/computer engineering</c:v>
+                  <c:v>Cell/molecular biology</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>Cell/molecular biology</c:v>
+                  <c:v> Agricultural/food sciences</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v> Agricultural/food sciences</c:v>
+                  <c:v>Other social sciences</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>Other social sciences</c:v>
+                  <c:v>Economics</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>Economics</c:v>
+                  <c:v>Computer/information sciences</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>Computer/information sciences</c:v>
+                  <c:v>Psychology</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>Psychology</c:v>
+                  <c:v>Physics</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>Physics</c:v>
+                  <c:v>Other engineering</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>Other engineering</c:v>
+                  <c:v> Biochemistry/biophysics</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v> Biochemistry/biophysics</c:v>
+                  <c:v>Chemistry, except biochemistry</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>Chemistry, except biochemistry</c:v>
+                  <c:v>Health</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>Health</c:v>
+                  <c:v>Astronomy/astrophysics</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>Astronomy/astrophysics</c:v>
+                  <c:v>Other biological sciences</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>Other biological sciences</c:v>
+                  <c:v>Civil engineering</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>Civil engineering</c:v>
+                  <c:v>Earth/atmospheric/ocean sciencesd</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>Earth/atmospheric/ocean sciencesd</c:v>
+                  <c:v> Microbiology</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v> Microbiology</c:v>
+                  <c:v>Environmental life sciences</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>Environmental life sciences</c:v>
-                </c:pt>
-                <c:pt idx="26">
                   <c:v> Zoology</c:v>
                 </c:pt>
               </c:strCache>
@@ -8136,94 +8190,99 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet6!$C$39:$C$65</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Graph Data Analysis Tables'!$C$39:$C$65</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'Graph Data Analysis Tables'!$C$40:$C$65</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.75200442355543273</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.75200442355543273</c:v>
+                  <c:v>0.97318219518938343</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.97318219518938343</c:v>
+                  <c:v>1.0881946364390378</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.0881946364390378</c:v>
+                  <c:v>0.78739286701686484</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>0.98202930605474148</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.81393419961293889</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.98202930605474148</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0616533038429639</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>0.78739286701686484</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.98202930605474148</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.81393419961293889</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.98202930605474148</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.0616533038429639</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0.78739286701686484</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.78739286701686484</c:v>
+                  <c:v>0.68122753663256841</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.68122753663256841</c:v>
+                  <c:v>1.04395908211225</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.04395908211225</c:v>
+                  <c:v>0.99972352778545759</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.99972352778545759</c:v>
+                  <c:v>0.76969864528614873</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.76969864528614873</c:v>
+                  <c:v>0.8847110865358031</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>0.8847110865358031</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.8847110865358031</c:v>
+                  <c:v>0.831628421343655</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.831628421343655</c:v>
+                  <c:v>0.85816975393972905</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.85816975393972905</c:v>
+                  <c:v>0.84047553220901294</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.84047553220901294</c:v>
+                  <c:v>0.74315731269007468</c:v>
                 </c:pt>
                 <c:pt idx="20">
+                  <c:v>0.75200442355543273</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.82278131047829695</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.76085153442079068</c:v>
+                </c:pt>
+                <c:pt idx="23">
                   <c:v>0.74315731269007468</c:v>
                 </c:pt>
-                <c:pt idx="21">
-                  <c:v>0.75200442355543273</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0.82278131047829695</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>0.76085153442079068</c:v>
-                </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.74315731269007468</c:v>
+                  <c:v>0.66353331490185241</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.66353331490185241</c:v>
-                </c:pt>
-                <c:pt idx="26">
                   <c:v>0.63699198230577825</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-44FD-4F08-A61E-5684726D87CA}"/>
@@ -8235,7 +8294,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet6!$H$39</c:f>
+              <c:f>'Graph Data Analysis Tables'!$H$39</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -8245,102 +8304,209 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent6"/>
-            </a:solidFill>
-            <a:ln w="25400">
-              <a:noFill/>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="26"/>
+              <c:pt idx="0">
+                <c:v>Sociology</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>Mechanical engineering</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>Aerospace/aeronautical/astronautical engineering</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>Political sciences</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>Materials and metallurgical engineering</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>Mathematics/statistics</c:v>
+              </c:pt>
+              <c:pt idx="6">
+                <c:v>Chemical engineering</c:v>
+              </c:pt>
+              <c:pt idx="7">
+                <c:v>Electrical/computer engineering</c:v>
+              </c:pt>
+              <c:pt idx="8">
+                <c:v>Cell/molecular biology</c:v>
+              </c:pt>
+              <c:pt idx="9">
+                <c:v> Agricultural/food sciences</c:v>
+              </c:pt>
+              <c:pt idx="10">
+                <c:v>Other social sciences</c:v>
+              </c:pt>
+              <c:pt idx="11">
+                <c:v>Economics</c:v>
+              </c:pt>
+              <c:pt idx="12">
+                <c:v>Computer/information sciences</c:v>
+              </c:pt>
+              <c:pt idx="13">
+                <c:v>Psychology</c:v>
+              </c:pt>
+              <c:pt idx="14">
+                <c:v>Physics</c:v>
+              </c:pt>
+              <c:pt idx="15">
+                <c:v>Other engineering</c:v>
+              </c:pt>
+              <c:pt idx="16">
+                <c:v> Biochemistry/biophysics</c:v>
+              </c:pt>
+              <c:pt idx="17">
+                <c:v>Chemistry, except biochemistry</c:v>
+              </c:pt>
+              <c:pt idx="18">
+                <c:v>Health</c:v>
+              </c:pt>
+              <c:pt idx="19">
+                <c:v>Astronomy/astrophysics</c:v>
+              </c:pt>
+              <c:pt idx="20">
+                <c:v>Other biological sciences</c:v>
+              </c:pt>
+              <c:pt idx="21">
+                <c:v>Civil engineering</c:v>
+              </c:pt>
+              <c:pt idx="22">
+                <c:v>Earth/atmospheric/ocean sciencesd</c:v>
+              </c:pt>
+              <c:pt idx="23">
+                <c:v> Microbiology</c:v>
+              </c:pt>
+              <c:pt idx="24">
+                <c:v>Environmental life sciences</c:v>
+              </c:pt>
+              <c:pt idx="25">
+                <c:v> Zoology</c:v>
+              </c:pt>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:autoCat val="1"/>
+                </c:ext>
+              </c:extLst>
+            </c:strLit>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet6!$H$40:$H$65</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Graph Data Analysis Tables'!$H$40:$H$65</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'Graph Data Analysis Tables'!$H$41:$H$65</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="0">
-                  <c:v>0.79623997788222278</c:v>
+                  <c:v>1.0439590821122477</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0439590821122477</c:v>
+                  <c:v>1.1678186342272601</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.1678186342272601</c:v>
+                  <c:v>0.85816975393972905</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.85816975393972905</c:v>
+                  <c:v>1.1058888581697539</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.1058888581697539</c:v>
+                  <c:v>0.92894664086259326</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.92894664086259326</c:v>
+                  <c:v>1.1412773016311861</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.1412773016311861</c:v>
+                  <c:v>1.2385955211501245</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.2385955211501245</c:v>
+                  <c:v>0.92009952999723532</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0.92009952999723532</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>0.79623997788222278</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.2297484102847664</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.1855128559579762</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>0.92009952999723532</c:v>
                 </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.79623997788222278</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1.2297484102847664</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1.1855128559579762</c:v>
-                </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.92009952999723532</c:v>
+                  <c:v>1.0616533038429639</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>1.0616533038429639</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.0616533038429639</c:v>
+                  <c:v>1.0085706386508155</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.0085706386508155</c:v>
+                  <c:v>1.0439590821122477</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.0439590821122477</c:v>
+                  <c:v>1.0262648603815316</c:v>
                 </c:pt>
                 <c:pt idx="18">
+                  <c:v>0.91125241913187727</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.92894664086259326</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>1.0262648603815316</c:v>
                 </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.91125241913187727</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0.92894664086259326</c:v>
-                </c:pt>
                 <c:pt idx="21">
-                  <c:v>1.0262648603815316</c:v>
+                  <c:v>0.95548797345866743</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.95548797345866743</c:v>
+                  <c:v>0.97318219518938343</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.97318219518938343</c:v>
+                  <c:v>0.87586397567044516</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.87586397567044516</c:v>
-                </c:pt>
-                <c:pt idx="25">
                   <c:v>0.849322643074371</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000005-44FD-4F08-A61E-5684726D87CA}"/>
@@ -8355,12 +8521,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="150"/>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
         <c:axId val="1937504240"/>
         <c:axId val="1950462736"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-            <c15:filteredBarSeries>
+            <c15:filteredLineSeries>
               <c15:ser>
                 <c:idx val="0"/>
                 <c:order val="0"/>
@@ -8369,7 +8536,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Sheet6!$B$39</c15:sqref>
+                          <c15:sqref>'Graph Data Analysis Tables'!$B$39</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -8382,105 +8549,119 @@
                   </c:strRef>
                 </c:tx>
                 <c:spPr>
-                  <a:solidFill>
-                    <a:schemeClr val="accent1"/>
-                  </a:solidFill>
-                  <a:ln w="25400">
-                    <a:noFill/>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:round/>
                   </a:ln>
                   <a:effectLst/>
                 </c:spPr>
-                <c:invertIfNegative val="0"/>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent1"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
                 <c:cat>
                   <c:strRef>
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref>'Graph Data Analysis Tables'!$A$39:$A$65</c15:sqref>
+                        </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>Sheet6!$A$39:$A$65</c15:sqref>
+                          <c15:sqref>'Graph Data Analysis Tables'!$A$40:$A$65</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:strCache>
-                      <c:ptCount val="27"/>
+                      <c:ptCount val="26"/>
                       <c:pt idx="0">
-                        <c:v>Row Labels</c:v>
+                        <c:v>Sociology</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>Sociology</c:v>
+                        <c:v>Mechanical engineering</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>Mechanical engineering</c:v>
+                        <c:v>Aerospace/aeronautical/astronautical engineering</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>Aerospace/aeronautical/astronautical engineering</c:v>
+                        <c:v>Political sciences</c:v>
                       </c:pt>
                       <c:pt idx="4">
-                        <c:v>Political sciences</c:v>
+                        <c:v>Materials and metallurgical engineering</c:v>
                       </c:pt>
                       <c:pt idx="5">
-                        <c:v>Materials and metallurgical engineering</c:v>
+                        <c:v>Mathematics/statistics</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>Mathematics/statistics</c:v>
+                        <c:v>Chemical engineering</c:v>
                       </c:pt>
                       <c:pt idx="7">
-                        <c:v>Chemical engineering</c:v>
+                        <c:v>Electrical/computer engineering</c:v>
                       </c:pt>
                       <c:pt idx="8">
-                        <c:v>Electrical/computer engineering</c:v>
+                        <c:v>Cell/molecular biology</c:v>
                       </c:pt>
                       <c:pt idx="9">
-                        <c:v>Cell/molecular biology</c:v>
+                        <c:v> Agricultural/food sciences</c:v>
                       </c:pt>
                       <c:pt idx="10">
-                        <c:v> Agricultural/food sciences</c:v>
+                        <c:v>Other social sciences</c:v>
                       </c:pt>
                       <c:pt idx="11">
-                        <c:v>Other social sciences</c:v>
+                        <c:v>Economics</c:v>
                       </c:pt>
                       <c:pt idx="12">
-                        <c:v>Economics</c:v>
+                        <c:v>Computer/information sciences</c:v>
                       </c:pt>
                       <c:pt idx="13">
-                        <c:v>Computer/information sciences</c:v>
+                        <c:v>Psychology</c:v>
                       </c:pt>
                       <c:pt idx="14">
-                        <c:v>Psychology</c:v>
+                        <c:v>Physics</c:v>
                       </c:pt>
                       <c:pt idx="15">
-                        <c:v>Physics</c:v>
+                        <c:v>Other engineering</c:v>
                       </c:pt>
                       <c:pt idx="16">
-                        <c:v>Other engineering</c:v>
+                        <c:v> Biochemistry/biophysics</c:v>
                       </c:pt>
                       <c:pt idx="17">
-                        <c:v> Biochemistry/biophysics</c:v>
+                        <c:v>Chemistry, except biochemistry</c:v>
                       </c:pt>
                       <c:pt idx="18">
-                        <c:v>Chemistry, except biochemistry</c:v>
+                        <c:v>Health</c:v>
                       </c:pt>
                       <c:pt idx="19">
-                        <c:v>Health</c:v>
+                        <c:v>Astronomy/astrophysics</c:v>
                       </c:pt>
                       <c:pt idx="20">
-                        <c:v>Astronomy/astrophysics</c:v>
+                        <c:v>Other biological sciences</c:v>
                       </c:pt>
                       <c:pt idx="21">
-                        <c:v>Other biological sciences</c:v>
+                        <c:v>Civil engineering</c:v>
                       </c:pt>
                       <c:pt idx="22">
-                        <c:v>Civil engineering</c:v>
+                        <c:v>Earth/atmospheric/ocean sciencesd</c:v>
                       </c:pt>
                       <c:pt idx="23">
-                        <c:v>Earth/atmospheric/ocean sciencesd</c:v>
+                        <c:v> Microbiology</c:v>
                       </c:pt>
                       <c:pt idx="24">
-                        <c:v> Microbiology</c:v>
+                        <c:v>Environmental life sciences</c:v>
                       </c:pt>
                       <c:pt idx="25">
-                        <c:v>Environmental life sciences</c:v>
-                      </c:pt>
-                      <c:pt idx="26">
                         <c:v> Zoology</c:v>
                       </c:pt>
                     </c:strCache>
@@ -8490,106 +8671,107 @@
                   <c:numRef>
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref>'Graph Data Analysis Tables'!$B$39:$B$65</c15:sqref>
+                        </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>Sheet6!$B$39:$B$65</c15:sqref>
+                          <c15:sqref>'Graph Data Analysis Tables'!$B$40:$B$65</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="27"/>
+                      <c:ptCount val="26"/>
                       <c:pt idx="0">
-                        <c:v>0</c:v>
+                        <c:v>0.94444444444444442</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>0.94444444444444442</c:v>
+                        <c:v>0.93220338983050843</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>0.93220338983050843</c:v>
+                        <c:v>0.93181818181818177</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>0.93181818181818177</c:v>
+                        <c:v>0.91752577319587625</c:v>
                       </c:pt>
                       <c:pt idx="4">
-                        <c:v>0.91752577319587625</c:v>
+                        <c:v>0.88800000000000001</c:v>
                       </c:pt>
                       <c:pt idx="5">
-                        <c:v>0.88800000000000001</c:v>
+                        <c:v>0.87619047619047619</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>0.87619047619047619</c:v>
+                        <c:v>0.86046511627906974</c:v>
                       </c:pt>
                       <c:pt idx="7">
-                        <c:v>0.86046511627906974</c:v>
+                        <c:v>0.8571428571428571</c:v>
                       </c:pt>
                       <c:pt idx="8">
-                        <c:v>0.8571428571428571</c:v>
+                        <c:v>0.85576923076923073</c:v>
                       </c:pt>
                       <c:pt idx="9">
                         <c:v>0.85576923076923073</c:v>
                       </c:pt>
                       <c:pt idx="10">
-                        <c:v>0.85576923076923073</c:v>
+                        <c:v>0.85555555555555551</c:v>
                       </c:pt>
                       <c:pt idx="11">
-                        <c:v>0.85555555555555551</c:v>
+                        <c:v>0.84892086330935257</c:v>
                       </c:pt>
                       <c:pt idx="12">
-                        <c:v>0.84892086330935257</c:v>
+                        <c:v>0.84328358208955223</c:v>
                       </c:pt>
                       <c:pt idx="13">
-                        <c:v>0.84328358208955223</c:v>
+                        <c:v>0.83653846153846156</c:v>
                       </c:pt>
                       <c:pt idx="14">
-                        <c:v>0.83653846153846156</c:v>
+                        <c:v>0.83333333333333337</c:v>
                       </c:pt>
                       <c:pt idx="15">
                         <c:v>0.83333333333333337</c:v>
                       </c:pt>
                       <c:pt idx="16">
-                        <c:v>0.83333333333333337</c:v>
+                        <c:v>0.82456140350877194</c:v>
                       </c:pt>
                       <c:pt idx="17">
-                        <c:v>0.82456140350877194</c:v>
+                        <c:v>0.82203389830508478</c:v>
                       </c:pt>
                       <c:pt idx="18">
-                        <c:v>0.82203389830508478</c:v>
+                        <c:v>0.81896551724137934</c:v>
                       </c:pt>
                       <c:pt idx="19">
-                        <c:v>0.81896551724137934</c:v>
+                        <c:v>0.81553398058252424</c:v>
                       </c:pt>
                       <c:pt idx="20">
-                        <c:v>0.81553398058252424</c:v>
+                        <c:v>0.80952380952380953</c:v>
                       </c:pt>
                       <c:pt idx="21">
-                        <c:v>0.80952380952380953</c:v>
+                        <c:v>0.80172413793103448</c:v>
                       </c:pt>
                       <c:pt idx="22">
-                        <c:v>0.80172413793103448</c:v>
+                        <c:v>0.79629629629629628</c:v>
                       </c:pt>
                       <c:pt idx="23">
-                        <c:v>0.79629629629629628</c:v>
+                        <c:v>0.76363636363636367</c:v>
                       </c:pt>
                       <c:pt idx="24">
-                        <c:v>0.76363636363636367</c:v>
+                        <c:v>0.75757575757575757</c:v>
                       </c:pt>
                       <c:pt idx="25">
-                        <c:v>0.75757575757575757</c:v>
-                      </c:pt>
-                      <c:pt idx="26">
                         <c:v>0.75</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
+                <c:smooth val="0"/>
                 <c:extLst>
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000000-44FD-4F08-A61E-5684726D87CA}"/>
                   </c:ext>
                 </c:extLst>
               </c15:ser>
-            </c15:filteredBarSeries>
-            <c15:filteredBarSeries>
+            </c15:filteredLineSeries>
+            <c15:filteredLineSeries>
               <c15:ser>
                 <c:idx val="2"/>
                 <c:order val="2"/>
@@ -8598,7 +8780,7 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Sheet6!$E$39</c15:sqref>
+                          <c15:sqref>'Graph Data Analysis Tables'!$E$39</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -8611,116 +8793,131 @@
                   </c:strRef>
                 </c:tx>
                 <c:spPr>
-                  <a:solidFill>
-                    <a:schemeClr val="accent3"/>
-                  </a:solidFill>
-                  <a:ln w="25400">
-                    <a:noFill/>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent3"/>
+                    </a:solidFill>
+                    <a:round/>
                   </a:ln>
                   <a:effectLst/>
                 </c:spPr>
-                <c:invertIfNegative val="0"/>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent3"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent3"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
                 <c:val>
                   <c:numRef>
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref>'Graph Data Analysis Tables'!$E$40:$E$65</c15:sqref>
+                        </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>Sheet6!$E$40:$E$65</c15:sqref>
+                          <c15:sqref>'Graph Data Analysis Tables'!$E$41:$E$65</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="26"/>
+                      <c:ptCount val="25"/>
                       <c:pt idx="0">
-                        <c:v>90000</c:v>
+                        <c:v>118000</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>118000</c:v>
+                        <c:v>132000</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>132000</c:v>
+                        <c:v>97000</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>97000</c:v>
+                        <c:v>125000</c:v>
                       </c:pt>
                       <c:pt idx="4">
-                        <c:v>125000</c:v>
+                        <c:v>105000</c:v>
                       </c:pt>
                       <c:pt idx="5">
-                        <c:v>105000</c:v>
+                        <c:v>129000</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>129000</c:v>
+                        <c:v>140000</c:v>
                       </c:pt>
                       <c:pt idx="7">
-                        <c:v>140000</c:v>
+                        <c:v>104000</c:v>
                       </c:pt>
                       <c:pt idx="8">
                         <c:v>104000</c:v>
                       </c:pt>
                       <c:pt idx="9">
+                        <c:v>90000</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>139000</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>134000</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
                         <c:v>104000</c:v>
                       </c:pt>
-                      <c:pt idx="10">
-                        <c:v>90000</c:v>
-                      </c:pt>
-                      <c:pt idx="11">
-                        <c:v>139000</c:v>
-                      </c:pt>
-                      <c:pt idx="12">
-                        <c:v>134000</c:v>
-                      </c:pt>
                       <c:pt idx="13">
-                        <c:v>104000</c:v>
+                        <c:v>120000</c:v>
                       </c:pt>
                       <c:pt idx="14">
                         <c:v>120000</c:v>
                       </c:pt>
                       <c:pt idx="15">
-                        <c:v>120000</c:v>
+                        <c:v>114000</c:v>
                       </c:pt>
                       <c:pt idx="16">
-                        <c:v>114000</c:v>
+                        <c:v>118000</c:v>
                       </c:pt>
                       <c:pt idx="17">
-                        <c:v>118000</c:v>
+                        <c:v>116000</c:v>
                       </c:pt>
                       <c:pt idx="18">
+                        <c:v>103000</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>105000</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
                         <c:v>116000</c:v>
                       </c:pt>
-                      <c:pt idx="19">
-                        <c:v>103000</c:v>
-                      </c:pt>
-                      <c:pt idx="20">
-                        <c:v>105000</c:v>
-                      </c:pt>
                       <c:pt idx="21">
-                        <c:v>116000</c:v>
+                        <c:v>108000</c:v>
                       </c:pt>
                       <c:pt idx="22">
-                        <c:v>108000</c:v>
+                        <c:v>110000</c:v>
                       </c:pt>
                       <c:pt idx="23">
-                        <c:v>110000</c:v>
+                        <c:v>99000</c:v>
                       </c:pt>
                       <c:pt idx="24">
-                        <c:v>99000</c:v>
-                      </c:pt>
-                      <c:pt idx="25">
                         <c:v>96000</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
+                <c:smooth val="0"/>
                 <c:extLst>
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000002-44FD-4F08-A61E-5684726D87CA}"/>
                   </c:ext>
                 </c:extLst>
               </c15:ser>
-            </c15:filteredBarSeries>
-            <c15:filteredBarSeries>
+            </c15:filteredLineSeries>
+            <c15:filteredLineSeries>
               <c15:ser>
                 <c:idx val="3"/>
                 <c:order val="3"/>
@@ -8729,7 +8926,7 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Sheet6!$F$39</c15:sqref>
+                          <c15:sqref>'Graph Data Analysis Tables'!$F$39</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -8742,116 +8939,131 @@
                   </c:strRef>
                 </c:tx>
                 <c:spPr>
-                  <a:solidFill>
-                    <a:schemeClr val="accent4"/>
-                  </a:solidFill>
-                  <a:ln w="25400">
-                    <a:noFill/>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent4"/>
+                    </a:solidFill>
+                    <a:round/>
                   </a:ln>
                   <a:effectLst/>
                 </c:spPr>
-                <c:invertIfNegative val="0"/>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent4"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent4"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
                 <c:val>
                   <c:numRef>
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref>'Graph Data Analysis Tables'!$F$40:$F$65</c15:sqref>
+                        </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>Sheet6!$F$40:$F$65</c15:sqref>
+                          <c15:sqref>'Graph Data Analysis Tables'!$F$41:$F$65</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="26"/>
+                      <c:ptCount val="25"/>
                       <c:pt idx="0">
-                        <c:v>85000</c:v>
+                        <c:v>110000</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>110000</c:v>
+                        <c:v>123000</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>123000</c:v>
+                        <c:v>89000</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>89000</c:v>
+                        <c:v>111000</c:v>
                       </c:pt>
                       <c:pt idx="4">
+                        <c:v>92000</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
                         <c:v>111000</c:v>
                       </c:pt>
-                      <c:pt idx="5">
-                        <c:v>92000</c:v>
-                      </c:pt>
                       <c:pt idx="6">
-                        <c:v>111000</c:v>
+                        <c:v>120000</c:v>
                       </c:pt>
                       <c:pt idx="7">
-                        <c:v>120000</c:v>
+                        <c:v>89000</c:v>
                       </c:pt>
                       <c:pt idx="8">
                         <c:v>89000</c:v>
                       </c:pt>
                       <c:pt idx="9">
-                        <c:v>89000</c:v>
+                        <c:v>77000</c:v>
                       </c:pt>
                       <c:pt idx="10">
-                        <c:v>77000</c:v>
+                        <c:v>118000</c:v>
                       </c:pt>
                       <c:pt idx="11">
-                        <c:v>118000</c:v>
+                        <c:v>113000</c:v>
                       </c:pt>
                       <c:pt idx="12">
-                        <c:v>113000</c:v>
+                        <c:v>87000</c:v>
                       </c:pt>
                       <c:pt idx="13">
-                        <c:v>87000</c:v>
+                        <c:v>100000</c:v>
                       </c:pt>
                       <c:pt idx="14">
                         <c:v>100000</c:v>
                       </c:pt>
                       <c:pt idx="15">
-                        <c:v>100000</c:v>
+                        <c:v>94000</c:v>
                       </c:pt>
                       <c:pt idx="16">
-                        <c:v>94000</c:v>
+                        <c:v>97000</c:v>
                       </c:pt>
                       <c:pt idx="17">
-                        <c:v>97000</c:v>
+                        <c:v>95000</c:v>
                       </c:pt>
                       <c:pt idx="18">
-                        <c:v>95000</c:v>
+                        <c:v>84000</c:v>
                       </c:pt>
                       <c:pt idx="19">
+                        <c:v>85000</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>93000</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>86000</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
                         <c:v>84000</c:v>
                       </c:pt>
-                      <c:pt idx="20">
-                        <c:v>85000</c:v>
-                      </c:pt>
-                      <c:pt idx="21">
-                        <c:v>93000</c:v>
-                      </c:pt>
-                      <c:pt idx="22">
-                        <c:v>86000</c:v>
-                      </c:pt>
                       <c:pt idx="23">
-                        <c:v>84000</c:v>
+                        <c:v>75000</c:v>
                       </c:pt>
                       <c:pt idx="24">
-                        <c:v>75000</c:v>
-                      </c:pt>
-                      <c:pt idx="25">
                         <c:v>72000</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
+                <c:smooth val="0"/>
                 <c:extLst>
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000003-44FD-4F08-A61E-5684726D87CA}"/>
                   </c:ext>
                 </c:extLst>
               </c15:ser>
-            </c15:filteredBarSeries>
-            <c15:filteredBarSeries>
+            </c15:filteredLineSeries>
+            <c15:filteredLineSeries>
               <c15:ser>
                 <c:idx val="4"/>
                 <c:order val="4"/>
@@ -8860,7 +9072,7 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Sheet6!$G$39</c15:sqref>
+                          <c15:sqref>'Graph Data Analysis Tables'!$G$39</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -8873,118 +9085,133 @@
                   </c:strRef>
                 </c:tx>
                 <c:spPr>
-                  <a:solidFill>
-                    <a:schemeClr val="accent5"/>
-                  </a:solidFill>
-                  <a:ln w="25400">
-                    <a:noFill/>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent5"/>
+                    </a:solidFill>
+                    <a:round/>
                   </a:ln>
                   <a:effectLst/>
                 </c:spPr>
-                <c:invertIfNegative val="0"/>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent5"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent5"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
                 <c:val>
                   <c:numRef>
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref>'Graph Data Analysis Tables'!$G$40:$G$65</c15:sqref>
+                        </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>Sheet6!$G$40:$G$65</c15:sqref>
+                          <c15:sqref>'Graph Data Analysis Tables'!$G$41:$G$65</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="26"/>
+                      <c:ptCount val="25"/>
                       <c:pt idx="0">
-                        <c:v>87000</c:v>
+                        <c:v>117000</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>117000</c:v>
+                        <c:v>132000</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>132000</c:v>
+                        <c:v>94000</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>94000</c:v>
+                        <c:v>122000</c:v>
                       </c:pt>
                       <c:pt idx="4">
-                        <c:v>122000</c:v>
+                        <c:v>100000</c:v>
                       </c:pt>
                       <c:pt idx="5">
+                        <c:v>125000</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>135000</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>98000</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
                         <c:v>100000</c:v>
                       </c:pt>
-                      <c:pt idx="6">
-                        <c:v>125000</c:v>
-                      </c:pt>
-                      <c:pt idx="7">
-                        <c:v>135000</c:v>
-                      </c:pt>
-                      <c:pt idx="8">
-                        <c:v>98000</c:v>
-                      </c:pt>
                       <c:pt idx="9">
-                        <c:v>100000</c:v>
+                        <c:v>83000</c:v>
                       </c:pt>
                       <c:pt idx="10">
-                        <c:v>83000</c:v>
+                        <c:v>129000</c:v>
                       </c:pt>
                       <c:pt idx="11">
-                        <c:v>129000</c:v>
+                        <c:v>130000</c:v>
                       </c:pt>
                       <c:pt idx="12">
-                        <c:v>130000</c:v>
+                        <c:v>93000</c:v>
                       </c:pt>
                       <c:pt idx="13">
-                        <c:v>93000</c:v>
+                        <c:v>120000</c:v>
                       </c:pt>
                       <c:pt idx="14">
                         <c:v>120000</c:v>
                       </c:pt>
                       <c:pt idx="15">
-                        <c:v>120000</c:v>
+                        <c:v>107000</c:v>
                       </c:pt>
                       <c:pt idx="16">
-                        <c:v>107000</c:v>
+                        <c:v>110000</c:v>
                       </c:pt>
                       <c:pt idx="17">
-                        <c:v>110000</c:v>
+                        <c:v>100000</c:v>
                       </c:pt>
                       <c:pt idx="18">
                         <c:v>100000</c:v>
                       </c:pt>
                       <c:pt idx="19">
+                        <c:v>97000</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>110000</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>102000</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
                         <c:v>100000</c:v>
                       </c:pt>
-                      <c:pt idx="20">
-                        <c:v>97000</c:v>
-                      </c:pt>
-                      <c:pt idx="21">
-                        <c:v>110000</c:v>
-                      </c:pt>
-                      <c:pt idx="22">
-                        <c:v>102000</c:v>
-                      </c:pt>
                       <c:pt idx="23">
-                        <c:v>100000</c:v>
+                        <c:v>90000</c:v>
                       </c:pt>
                       <c:pt idx="24">
-                        <c:v>90000</c:v>
-                      </c:pt>
-                      <c:pt idx="25">
                         <c:v>90000</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
+                <c:smooth val="0"/>
                 <c:extLst>
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000004-44FD-4F08-A61E-5684726D87CA}"/>
                   </c:ext>
                 </c:extLst>
               </c15:ser>
-            </c15:filteredBarSeries>
+            </c15:filteredLineSeries>
           </c:ext>
         </c:extLst>
-      </c:barChart>
+      </c:lineChart>
       <c:catAx>
         <c:axId val="1937504240"/>
         <c:scaling>
@@ -10280,16 +10507,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>114299</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>33131</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>24847</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>30</xdr:col>
-      <xdr:colOff>581024</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>572741</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>11595</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -10319,15 +10546,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>10328</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>176370</xdr:rowOff>
+      <xdr:colOff>2</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>27283</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>84</xdr:row>
-      <xdr:rowOff>132522</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>104776</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>73268</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -10360,7 +10587,7 @@
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Author" refreshedDate="43187.88169548611" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="32" xr:uid="{D6D2DAE5-9EFC-4174-9722-D2E37D897257}">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A57:G89" sheet="SDR2015_DST_50"/>
+    <worksheetSource ref="A57:G89" sheet="Raw_Data_Sheet"/>
   </cacheSource>
   <cacheFields count="7">
     <cacheField name="Field" numFmtId="0">
@@ -12615,8 +12842,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55AE6C91-E56D-4C1F-837C-09A02283502E}">
   <dimension ref="A1:N65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B27" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView topLeftCell="B21" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14254,7 +14481,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8013BB41-FAF9-45DD-ACFC-9292C0F87E5C}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A51" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
@@ -14269,8 +14496,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D465D0B9-A4C1-4290-9844-AD9374DA4E0F}">
   <dimension ref="A2:W160"/>
   <sheetViews>
-    <sheetView topLeftCell="A114" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I128" sqref="I128"/>
+    <sheetView tabSelected="1" topLeftCell="A130" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J160" sqref="J160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14287,6 +14514,7 @@
     <col min="18" max="19" width="20.140625" customWidth="1"/>
     <col min="20" max="20" width="24.42578125" customWidth="1"/>
     <col min="21" max="21" width="29.28515625" customWidth="1"/>
+    <col min="23" max="23" width="32" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">

</xml_diff>